<commit_message>
Added constraints to visit forms
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegan/app-designer/app/config/tables/visit/forms/visit/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="1760" windowWidth="23840" windowHeight="14300" tabRatio="500"/>
+    <workbookView xWindow="8720" yWindow="2980" windowWidth="41220" windowHeight="20640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -15,6 +20,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -23,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="122">
   <si>
     <t>setting_name</t>
   </si>
@@ -371,6 +379,24 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>constraint_message</t>
+  </si>
+  <si>
+    <t>The crop yield must be a positive value less than 8000 kg. Please enter a valid number.</t>
+  </si>
+  <si>
+    <t>The height of a maize plant must be a positive value less than 1100 cm. Please enter a valid number.</t>
+  </si>
+  <si>
+    <t>data('plant_height')  &gt;  0 &amp;&amp; data('plant_height') &lt; 1100</t>
+  </si>
+  <si>
+    <t>data('crop_yield') &gt; 0 &amp;&amp; data('crop_yield')  &lt;  8000</t>
   </si>
 </sst>
 </file>
@@ -1007,13 +1033,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
@@ -1021,10 +1047,12 @@
     <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="42.5" customWidth="1"/>
+    <col min="7" max="7" width="59.1640625" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
@@ -1046,8 +1074,14 @@
       <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="H1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -1062,7 +1096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1073,7 +1107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D4" s="1" t="s">
         <v>47</v>
       </c>
@@ -1083,14 +1117,20 @@
       <c r="G4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>87</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D6" s="1" t="s">
         <v>67</v>
       </c>
@@ -1104,7 +1144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>73</v>
@@ -1113,7 +1153,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="4"/>
       <c r="D8" s="1" t="s">
@@ -1123,13 +1163,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
         <v>73</v>
@@ -1138,7 +1178,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="4"/>
       <c r="D11" s="1" t="s">
@@ -1148,13 +1188,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
         <v>73</v>
@@ -1163,7 +1203,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="D14" s="1" t="s">
@@ -1173,19 +1213,19 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="16" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1196,13 +1236,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1216,7 +1256,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="4" t="s">
         <v>73</v>
@@ -1225,7 +1265,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="4"/>
       <c r="D21" s="1" t="s">
@@ -1235,13 +1275,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="B23" s="4" t="s">
         <v>73</v>
@@ -1250,7 +1290,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="4"/>
       <c r="D24" s="1" t="s">
@@ -1260,13 +1300,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="4" t="s">
         <v>73</v>
@@ -1275,7 +1315,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="4"/>
       <c r="D27" s="1" t="s">
@@ -1285,13 +1325,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
       <c r="B29" s="4" t="s">
         <v>73</v>
@@ -1300,7 +1340,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
       <c r="B30" s="4"/>
       <c r="D30" s="1" t="s">
@@ -1310,19 +1350,19 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
       <c r="B31" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
       <c r="B32" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="4:7">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1336,7 +1376,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="4:7">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
         <v>115</v>
       </c>
@@ -1346,8 +1386,14 @@
       <c r="G34" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="35" spans="4:7">
+      <c r="H34" t="s">
+        <v>121</v>
+      </c>
+      <c r="I34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1361,11 +1407,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1377,7 +1418,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
@@ -1385,7 +1426,7 @@
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1399,7 +1440,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1411,7 +1452,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1423,7 +1464,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1435,12 +1476,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1451,7 +1492,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>57</v>
       </c>
@@ -1463,7 +1504,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1474,12 +1515,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1491,7 +1532,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1503,7 +1544,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1515,7 +1556,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1530,11 +1571,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1543,10 +1579,10 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1557,7 +1593,7 @@
     <col min="7" max="7" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1580,7 +1616,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="52" customHeight="1">
+    <row r="2" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>48</v>
       </c>
@@ -1604,11 +1640,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1620,14 +1651,14 @@
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1638,7 +1669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1646,7 +1677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1654,7 +1685,7 @@
         <v>20140331</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1662,7 +1693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1670,7 +1701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>96</v>
       </c>
@@ -1681,11 +1712,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1697,14 +1723,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -1721,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1738,7 +1764,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1755,7 +1781,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1774,10 +1800,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed visit form crash when inputting letters instead of numbers for crop yield
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegan/Documents/app-designer/app/config/tables/visit/forms/visit/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="8720" yWindow="2980" windowWidth="41220" windowHeight="20640" tabRatio="500"/>
   </bookViews>
@@ -20,11 +15,11 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -378,9 +373,6 @@
     <t>["crop_yield","plot_id","date","plant_height","plant_health","plant_picture_uriFragment","pests","soil","observations"]</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>constraint</t>
   </si>
   <si>
@@ -397,6 +389,9 @@
   </si>
   <si>
     <t>data('plant_height')  &gt;=  0 &amp;&amp; data('plant_height') &lt; 1100</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -1036,10 +1031,10 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
@@ -1052,7 +1047,7 @@
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
@@ -1075,13 +1070,13 @@
         <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="11"/>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -1096,7 +1091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1107,7 +1102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="D4" s="1" t="s">
         <v>47</v>
       </c>
@@ -1118,19 +1113,19 @@
         <v>111</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
         <v>87</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="D6" s="1" t="s">
         <v>67</v>
       </c>
@@ -1144,7 +1139,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>73</v>
@@ -1153,7 +1148,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="12"/>
       <c r="B8" s="4"/>
       <c r="D8" s="1" t="s">
@@ -1163,13 +1158,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
         <v>73</v>
@@ -1178,7 +1173,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="4"/>
       <c r="D11" s="1" t="s">
@@ -1188,13 +1183,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
         <v>73</v>
@@ -1203,7 +1198,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="D14" s="1" t="s">
@@ -1213,19 +1208,19 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="12"/>
       <c r="B15" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="D17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1236,13 +1231,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="B18" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="D19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1256,7 +1251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="12"/>
       <c r="B20" s="4" t="s">
         <v>73</v>
@@ -1265,7 +1260,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="12"/>
       <c r="B21" s="4"/>
       <c r="D21" s="1" t="s">
@@ -1275,13 +1270,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="12"/>
       <c r="B22" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="12"/>
       <c r="B23" s="4" t="s">
         <v>73</v>
@@ -1290,7 +1285,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" s="4"/>
       <c r="D24" s="1" t="s">
@@ -1300,13 +1295,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A25" s="12"/>
       <c r="B25" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A26" s="12"/>
       <c r="B26" s="4" t="s">
         <v>73</v>
@@ -1315,7 +1310,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="12"/>
       <c r="B27" s="4"/>
       <c r="D27" s="1" t="s">
@@ -1325,13 +1320,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A28" s="12"/>
       <c r="B28" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="12"/>
       <c r="B29" s="4" t="s">
         <v>73</v>
@@ -1340,7 +1335,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="12"/>
       <c r="B30" s="4"/>
       <c r="D30" s="1" t="s">
@@ -1350,19 +1345,19 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="12"/>
       <c r="B31" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="12"/>
       <c r="B32" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:9">
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1376,9 +1371,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:9">
       <c r="D34" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="F34" t="s">
         <v>112</v>
@@ -1387,13 +1382,13 @@
         <v>113</v>
       </c>
       <c r="H34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I34" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9">
       <c r="D35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1407,6 +1402,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1418,7 +1418,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
@@ -1426,7 +1426,7 @@
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1476,12 +1476,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="10" t="s">
         <v>57</v>
       </c>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1515,12 +1515,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1571,6 +1571,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1582,7 +1587,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1593,7 +1598,7 @@
     <col min="7" max="7" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1616,7 +1621,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="52" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>48</v>
       </c>
@@ -1640,6 +1645,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1651,14 +1661,14 @@
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1677,7 +1687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1685,7 +1695,7 @@
         <v>20140331</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1693,7 +1703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1701,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="32">
       <c r="A6" s="13" t="s">
         <v>96</v>
       </c>
@@ -1712,6 +1722,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1723,14 +1738,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -1747,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1764,7 +1779,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1781,7 +1796,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1800,5 +1815,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added visit form requirements
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegan/Documents/app-designer/app/config/tables/visit/forms/visit/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="2980" windowWidth="41220" windowHeight="20640" tabRatio="500"/>
+    <workbookView xWindow="5960" yWindow="5320" windowWidth="41220" windowHeight="20640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -15,18 +20,18 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
   <si>
     <t>setting_name</t>
   </si>
@@ -392,6 +397,9 @@
   </si>
   <si>
     <t>integer</t>
+  </si>
+  <si>
+    <t>required</t>
   </si>
 </sst>
 </file>
@@ -1028,13 +1036,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
@@ -1047,7 +1055,7 @@
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
@@ -1075,8 +1083,11 @@
       <c r="I1" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1">
+      <c r="J1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -1090,8 +1101,11 @@
       <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1101,8 +1115,11 @@
       <c r="G3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D4" s="1" t="s">
         <v>47</v>
       </c>
@@ -1119,13 +1136,13 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>87</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D6" s="1" t="s">
         <v>67</v>
       </c>
@@ -1139,7 +1156,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>73</v>
@@ -1148,7 +1165,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="4"/>
       <c r="D8" s="1" t="s">
@@ -1158,13 +1175,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
         <v>73</v>
@@ -1173,7 +1190,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="4"/>
       <c r="D11" s="1" t="s">
@@ -1183,13 +1200,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
         <v>73</v>
@@ -1198,7 +1215,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="D14" s="1" t="s">
@@ -1208,19 +1225,19 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1231,13 +1248,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1251,7 +1268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="4" t="s">
         <v>73</v>
@@ -1260,7 +1277,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="4"/>
       <c r="D21" s="1" t="s">
@@ -1270,13 +1287,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="B23" s="4" t="s">
         <v>73</v>
@@ -1285,7 +1302,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="4"/>
       <c r="D24" s="1" t="s">
@@ -1295,13 +1312,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="4" t="s">
         <v>73</v>
@@ -1310,7 +1327,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="4"/>
       <c r="D27" s="1" t="s">
@@ -1320,13 +1337,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
       <c r="B29" s="4" t="s">
         <v>73</v>
@@ -1335,7 +1352,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
       <c r="B30" s="4"/>
       <c r="D30" s="1" t="s">
@@ -1345,19 +1362,19 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
       <c r="B31" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
       <c r="B32" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="4:9">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1371,7 +1388,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="4:9">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
         <v>121</v>
       </c>
@@ -1388,7 +1405,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="4:9">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1402,11 +1419,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1418,7 +1430,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
@@ -1426,7 +1438,7 @@
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1440,7 +1452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1464,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1464,7 +1476,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1476,12 +1488,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1492,7 +1504,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>57</v>
       </c>
@@ -1504,7 +1516,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1515,12 +1527,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1532,7 +1544,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1544,7 +1556,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1556,7 +1568,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1571,11 +1583,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1587,7 +1594,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1598,7 +1605,7 @@
     <col min="7" max="7" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1621,7 +1628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="52" customHeight="1">
+    <row r="2" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>48</v>
       </c>
@@ -1645,11 +1652,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1661,14 +1663,14 @@
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1687,7 +1689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1695,7 +1697,7 @@
         <v>20140331</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1703,7 +1705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1711,7 +1713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="32">
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>96</v>
       </c>
@@ -1722,11 +1724,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1738,14 +1735,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -1762,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1779,7 +1776,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1796,7 +1793,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1815,10 +1812,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added dynamic crop height and yield max warnings
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,14 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="5320" windowWidth="41220" windowHeight="20640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="50880" windowHeight="26400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="queries" sheetId="4" r:id="rId3"/>
-    <sheet name="settings" sheetId="3" r:id="rId4"/>
-    <sheet name="properties" sheetId="5" r:id="rId5"/>
+    <sheet name="prompt_types" sheetId="6" r:id="rId4"/>
+    <sheet name="calculates" sheetId="7" r:id="rId5"/>
+    <sheet name="model" sheetId="9" r:id="rId6"/>
+    <sheet name="settings" sheetId="3" r:id="rId7"/>
+    <sheet name="properties" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="165">
   <si>
     <t>setting_name</t>
   </si>
@@ -69,9 +72,6 @@
     <t>display.text</t>
   </si>
   <si>
-    <t>comments</t>
-  </si>
-  <si>
     <t>clause</t>
   </si>
   <si>
@@ -366,9 +366,6 @@
     <t>'plot_id&gt;='+opendatakit.encodeURIValue(0)</t>
   </si>
   <si>
-    <t>What is the height of the plant in cm?</t>
-  </si>
-  <si>
     <t>crop_yield</t>
   </si>
   <si>
@@ -384,22 +381,154 @@
     <t>constraint_message</t>
   </si>
   <si>
-    <t>The crop yield must be a positive value less than 8000 kg. Please enter a valid number.</t>
-  </si>
-  <si>
-    <t>The height of a maize plant must be a positive value less than 1100 cm. Please enter a valid number.</t>
-  </si>
-  <si>
-    <t>data('crop_yield') &gt;= 0 &amp;&amp; data('crop_yield')  &lt;  8000</t>
-  </si>
-  <si>
-    <t>data('plant_height')  &gt;=  0 &amp;&amp; data('plant_height') &lt; 1100</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
     <t>required</t>
+  </si>
+  <si>
+    <t>_savepoint_type = ?</t>
+  </si>
+  <si>
+    <t>['COMPLETE']</t>
+  </si>
+  <si>
+    <t>''</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>display.debug</t>
+  </si>
+  <si>
+    <t>async_assign_max</t>
+  </si>
+  <si>
+    <t>max_sample</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>prompt_type_name</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>async_assign_min</t>
+  </si>
+  <si>
+    <t>async_assign_avg</t>
+  </si>
+  <si>
+    <t>async_assign_sum</t>
+  </si>
+  <si>
+    <t>async_assign_total</t>
+  </si>
+  <si>
+    <t>async_assign_count</t>
+  </si>
+  <si>
+    <t>calculation_name</t>
+  </si>
+  <si>
+    <t>ack_ok</t>
+  </si>
+  <si>
+    <t>if // check_outlier</t>
+  </si>
+  <si>
+    <t>acknowledge</t>
+  </si>
+  <si>
+    <t>The height you have entered is an outlier.  Are you certain of this measurement?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>branch_label</t>
+  </si>
+  <si>
+    <t>survey_screen</t>
+  </si>
+  <si>
+    <t>goto survey_screen</t>
+  </si>
+  <si>
+    <t>display.hint</t>
+  </si>
+  <si>
+    <t>if // branch_fail</t>
+  </si>
+  <si>
+    <t>! data('ack_ok')</t>
+  </si>
+  <si>
+    <t>end if // branch_fail</t>
+  </si>
+  <si>
+    <t>end if // check_outlier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the height of the crop in cm? </t>
+  </si>
+  <si>
+    <t>isSessionVariable</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>fieldName</t>
+  </si>
+  <si>
+    <t>max_height</t>
+  </si>
+  <si>
+    <t>(data('plant_height') === null) ? false : ((data('plant_height') &gt;= 0) &amp;&amp; (data('plant_height') &lt;= (data('max_height') * 1.2)))</t>
+  </si>
+  <si>
+    <t>min_max_height</t>
+  </si>
+  <si>
+    <t>min_max_yield</t>
+  </si>
+  <si>
+    <t>max_yield</t>
+  </si>
+  <si>
+    <t>below_max_height</t>
+  </si>
+  <si>
+    <t>below_max_yield</t>
+  </si>
+  <si>
+    <t>(data('crop_yield') === null) ? false : ((data('crop_yield') &gt;= 0) &amp;&amp; (data('crop_yield') &lt;= (data('max_yield') * 1.2)))</t>
+  </si>
+  <si>
+    <t>! calculates.below_max_yield()</t>
+  </si>
+  <si>
+    <t>data('ack_ok') || calculates.below_max_yield()</t>
+  </si>
+  <si>
+    <t>! calculates.below_max_height()</t>
+  </si>
+  <si>
+    <t>data('ack_ok') || calculates.below_max_height()</t>
+  </si>
+  <si>
+    <t>The value you entered is outside of the current recorded range 0 thru {{data.max_height}}</t>
+  </si>
+  <si>
+    <t>The value you entered is outside of the current recorded range 0 thru {{data.max_yield}}</t>
   </si>
 </sst>
 </file>
@@ -450,18 +579,12 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -572,7 +695,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -584,10 +707,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -600,12 +723,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="91">
@@ -1036,384 +1180,859 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="59.1640625" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="76.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="10" width="59.1640625" customWidth="1"/>
+    <col min="11" max="11" width="50.5" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21"/>
+      <c r="B4" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21"/>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
+      <c r="B10" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" t="s">
+        <v>147</v>
+      </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
+      <c r="B12" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="M13" s="14"/>
+      <c r="N13" s="15"/>
+      <c r="P13" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+    </row>
+    <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+    </row>
+    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+    </row>
+    <row r="19" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21"/>
+      <c r="B21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21"/>
+      <c r="B22" s="4"/>
+      <c r="D22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21"/>
+      <c r="B23" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21"/>
+      <c r="B24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21"/>
+      <c r="B25" s="4"/>
+      <c r="D25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="21"/>
+      <c r="B26" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="21"/>
+      <c r="B27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
+      <c r="B28" s="4"/>
+      <c r="D28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="21"/>
+      <c r="B29" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="21"/>
+      <c r="B30" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="21"/>
+      <c r="B34" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="21"/>
+      <c r="B35" s="4"/>
+      <c r="D35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="21"/>
+      <c r="B36" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="21"/>
+      <c r="B37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="21"/>
+      <c r="B38" s="4"/>
+      <c r="D38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+      <c r="B39" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="21"/>
+      <c r="B40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="21"/>
+      <c r="B41" s="4"/>
+      <c r="D41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="21"/>
+      <c r="B42" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="21"/>
+      <c r="B43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="21"/>
+      <c r="B44" s="4"/>
+      <c r="D44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="21"/>
+      <c r="B45" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="21"/>
+      <c r="B46" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="21"/>
+      <c r="B47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="21"/>
+      <c r="B48" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" t="s">
+        <v>56</v>
+      </c>
+      <c r="I49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="21"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="14"/>
+      <c r="P50" s="14"/>
+    </row>
+    <row r="51" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="21"/>
+      <c r="B51" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E52" t="s">
+        <v>110</v>
+      </c>
+      <c r="I52" t="s">
+        <v>111</v>
+      </c>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+    </row>
+    <row r="53" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="21"/>
+      <c r="B53" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+    </row>
+    <row r="54" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="21"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="K54" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="M54" s="14"/>
+      <c r="N54" s="15"/>
+      <c r="P54" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+    </row>
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="14"/>
+    </row>
+    <row r="57" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="14"/>
+    </row>
+    <row r="58" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="14"/>
+      <c r="B58" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="14"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D59" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="4"/>
-      <c r="D8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="4"/>
-      <c r="D11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="D14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="4"/>
-      <c r="D21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="4"/>
-      <c r="D24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="4"/>
-      <c r="D27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
-      <c r="B29" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="4"/>
-      <c r="D30" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="E59" t="s">
         <v>33</v>
       </c>
-      <c r="G33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D34" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F34" t="s">
-        <v>112</v>
-      </c>
-      <c r="G34" t="s">
-        <v>113</v>
-      </c>
-      <c r="H34" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="I59" t="s">
         <v>34</v>
-      </c>
-      <c r="G35" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1440,52 +2059,52 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1495,36 +2114,36 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1534,50 +2153,50 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1588,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1600,53 +2219,109 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.5" customWidth="1"/>
-    <col min="7" max="7" width="43.1640625" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>110</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1656,6 +2331,176 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="170.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="22" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1707,15 +2552,15 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>96</v>
+      <c r="A6" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="B6" s="2" t="b">
         <v>1</v>
@@ -1727,7 +2572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1744,13 +2589,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>99</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1761,53 +2606,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
         <v>100</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
         <v>100</v>
       </c>
-      <c r="B3" t="s">
-        <v>101</v>
-      </c>
       <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
         <v>104</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>105</v>
-      </c>
-      <c r="E3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
       </c>
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
       <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
         <v>107</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>108</v>
-      </c>
-      <c r="E4" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plot demo comparison feature addition and style fixes
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="50880" windowHeight="26400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="50880" windowHeight="26400" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="174">
   <si>
     <t>setting_name</t>
   </si>
@@ -372,9 +372,6 @@
     <t>What is the current crop yield in kg per hectare?</t>
   </si>
   <si>
-    <t>["crop_yield","plot_id","date","plant_height","plant_health","plant_picture_uriFragment","pests","soil","observations"]</t>
-  </si>
-  <si>
     <t>constraint</t>
   </si>
   <si>
@@ -529,6 +526,36 @@
   </si>
   <si>
     <t>The value you entered is outside of the current recorded range 0 thru {{data.max_yield}}</t>
+  </si>
+  <si>
+    <t>plant_type</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>maize</t>
+  </si>
+  <si>
+    <t>What type of maize is grown at this plot?</t>
+  </si>
+  <si>
+    <t>["plot_id","plant_type","crop_yield","date","plant_height","plant_health","plant_picture_uriFragment","pests","soil","observations"]</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1203,7 +1230,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>12</v>
@@ -1221,25 +1248,25 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1247,14 +1274,14 @@
       <c r="B2" s="14"/>
       <c r="C2" s="16"/>
       <c r="D2" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
@@ -1271,14 +1298,14 @@
       <c r="B3" s="14"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -1293,7 +1320,7 @@
     <row r="4" spans="1:16" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21"/>
       <c r="B4" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="20"/>
@@ -1312,7 +1339,7 @@
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="20"/>
@@ -1350,63 +1377,59 @@
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="I7" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
+      <c r="B8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>26</v>
       </c>
-      <c r="M8" t="b">
+      <c r="M9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
-      <c r="B10" s="14" t="s">
-        <v>87</v>
-      </c>
+      <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>152</v>
+      </c>
       <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14" t="b">
+        <v>0</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -1416,97 +1439,98 @@
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D11" s="1" t="s">
+    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
+      <c r="B11" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="I11" t="s">
-        <v>147</v>
-      </c>
-      <c r="M11" t="b">
+      <c r="I12" t="s">
+        <v>146</v>
+      </c>
+      <c r="M12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-    </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="B13" s="14" t="s">
         <v>134</v>
       </c>
+      <c r="C13" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>162</v>
-      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="15"/>
-      <c r="P13" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>133</v>
+      </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-    </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="M14" s="14"/>
+      <c r="N14" s="15"/>
+      <c r="P14" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="14"/>
+        <v>142</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>143</v>
+      </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1520,10 +1544,10 @@
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
     </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="14" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -1542,7 +1566,7 @@
     <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -1560,7 +1584,9 @@
     </row>
     <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="B18" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -1575,305 +1601,302 @@
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+    </row>
+    <row r="20" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>41</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>49</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21"/>
-      <c r="B22" s="4"/>
-      <c r="D22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>79</v>
+      <c r="B22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21"/>
-      <c r="B23" s="4" t="s">
-        <v>75</v>
+      <c r="B23" s="4"/>
+      <c r="D23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21"/>
       <c r="B24" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21"/>
-      <c r="B25" s="4"/>
-      <c r="D25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>80</v>
+      <c r="B25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21"/>
-      <c r="B26" s="4" t="s">
-        <v>77</v>
+      <c r="B26" s="4"/>
+      <c r="D26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21"/>
       <c r="B27" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21"/>
-      <c r="B28" s="4"/>
-      <c r="D28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>81</v>
+      <c r="B28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21"/>
-      <c r="B29" s="4" t="s">
-        <v>77</v>
+      <c r="B29" s="4"/>
+      <c r="D29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21"/>
       <c r="B30" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="21"/>
+      <c r="B31" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D31" s="1" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D32" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>53</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I32" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B32" s="4" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>31</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F34" t="s">
         <v>40</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
-      <c r="B34" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21"/>
-      <c r="B35" s="4"/>
-      <c r="D35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>88</v>
+      <c r="B35" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="21"/>
-      <c r="B36" s="4" t="s">
-        <v>77</v>
+      <c r="B36" s="4"/>
+      <c r="D36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21"/>
       <c r="B37" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21"/>
-      <c r="B38" s="4"/>
-      <c r="D38" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>89</v>
+      <c r="B38" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="21"/>
-      <c r="B39" s="4" t="s">
-        <v>77</v>
+      <c r="B39" s="4"/>
+      <c r="D39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="21"/>
       <c r="B40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="21"/>
-      <c r="B41" s="4"/>
-      <c r="D41" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>90</v>
+      <c r="B41" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="21"/>
-      <c r="B42" s="4" t="s">
-        <v>75</v>
+      <c r="B42" s="4"/>
+      <c r="D42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="21"/>
       <c r="B43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21"/>
-      <c r="B44" s="4"/>
-      <c r="D44" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>91</v>
+      <c r="B44" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="21"/>
-      <c r="B45" s="4" t="s">
-        <v>75</v>
+      <c r="B45" s="4"/>
+      <c r="D45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21"/>
       <c r="B46" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21"/>
-      <c r="B47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="21"/>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="4"/>
+    </row>
+    <row r="49" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="21"/>
+      <c r="B49" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D49" s="1" t="s">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D50" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>32</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>56</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I50" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="21"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="15"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
     </row>
     <row r="51" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="21"/>
-      <c r="B51" s="14" t="s">
-        <v>87</v>
-      </c>
+      <c r="B51" s="14"/>
       <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="D51" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>153</v>
+      </c>
       <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
+      <c r="H51" s="14" t="b">
+        <v>0</v>
+      </c>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
       <c r="K51" s="14"/>
@@ -1883,96 +1906,97 @@
       <c r="O51" s="14"/>
       <c r="P51" s="14"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D52" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E52" t="s">
-        <v>110</v>
-      </c>
-      <c r="I52" t="s">
-        <v>111</v>
-      </c>
+    <row r="52" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+      <c r="B52" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
       <c r="J52" s="14"/>
       <c r="K52" s="14"/>
-    </row>
-    <row r="53" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
-      <c r="B53" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D53" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E53" t="s">
+        <v>110</v>
+      </c>
+      <c r="I53" t="s">
+        <v>111</v>
+      </c>
       <c r="J53" s="14"/>
       <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
-    </row>
-    <row r="54" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="21"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E54" s="14" t="s">
+      <c r="B54" s="14" t="s">
         <v>134</v>
       </c>
+      <c r="C54" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
       <c r="H54" s="14"/>
-      <c r="I54" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="J54" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="K54" s="14" t="s">
-        <v>160</v>
-      </c>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
       <c r="M54" s="14"/>
       <c r="N54" s="15"/>
-      <c r="P54" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+    </row>
+    <row r="55" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="21"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>133</v>
+      </c>
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
       <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-    </row>
-    <row r="56" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I55" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K55" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="M55" s="14"/>
+      <c r="N55" s="15"/>
+      <c r="P55" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
       <c r="B56" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C56" s="14"/>
+        <v>142</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>143</v>
+      </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
@@ -1986,10 +2010,10 @@
       <c r="N56" s="14"/>
       <c r="O56" s="14"/>
     </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="14" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
@@ -2008,7 +2032,7 @@
     <row r="58" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
       <c r="B58" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
@@ -2024,14 +2048,33 @@
       <c r="N58" s="14"/>
       <c r="O58" s="14"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D59" s="1" t="s">
+    <row r="59" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="14"/>
+      <c r="B59" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="14"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D60" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
         <v>33</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I60" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2043,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2197,6 +2240,39 @@
       <c r="C13" s="3"/>
       <c r="D13" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2244,7 +2320,7 @@
         <v>20</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>50</v>
@@ -2274,7 +2350,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -2286,21 +2362,21 @@
         <v>6</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>118</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -2312,16 +2388,16 @@
         <v>6</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>118</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>110</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2346,7 +2422,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -2354,50 +2430,50 @@
     </row>
     <row r="2" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2421,26 +2497,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
         <v>157</v>
-      </c>
-      <c r="B3" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2470,15 +2546,15 @@
         <v>8</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -2486,10 +2562,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -2576,15 +2652,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="5" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="138.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -2618,7 +2695,7 @@
         <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add async_assign_single_string custom prompt and use it to assign maize type
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegan/Documents/app-designer/app/config/tables/visit/forms/visit/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="50880" windowHeight="26400" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="10340" yWindow="1760" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,18 +18,18 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="179">
   <si>
     <t>setting_name</t>
   </si>
@@ -339,12 +334,6 @@
     <t>default</t>
   </si>
   <si>
-    <t>colOrder</t>
-  </si>
-  <si>
-    <t>array</t>
-  </si>
-  <si>
     <t>defaultViewType</t>
   </si>
   <si>
@@ -555,7 +544,28 @@
     <t>What type of maize is grown at this plot?</t>
   </si>
   <si>
-    <t>["plot_id","plant_type","crop_yield","date","plant_height","plant_health","plant_picture_uriFragment","pests","soil","observations"]</t>
+    <t>async_assign_single_string</t>
+  </si>
+  <si>
+    <t>plant_type_query_text</t>
+  </si>
+  <si>
+    <t>plant_type_query</t>
+  </si>
+  <si>
+    <t>_id = ?</t>
+  </si>
+  <si>
+    <t>[data('plot_id')]</t>
+  </si>
+  <si>
+    <t>planting</t>
+  </si>
+  <si>
+    <t>'plot_id='+opendatakit.encodeURIDataElement('plot_id')</t>
+  </si>
+  <si>
+    <t>data('plant_type_query_text')</t>
   </si>
 </sst>
 </file>
@@ -629,7 +639,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -721,8 +731,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -778,8 +790,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -825,6 +838,7 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -870,6 +884,7 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1207,13 +1222,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
@@ -1228,9 +1243,9 @@
     <col min="12" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>12</v>
@@ -1248,40 +1263,40 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A2" s="21"/>
       <c r="B2" s="14"/>
       <c r="C2" s="16"/>
       <c r="D2" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
@@ -1293,19 +1308,19 @@
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="21"/>
       <c r="B3" s="14"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -1317,10 +1332,10 @@
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A4" s="21"/>
       <c r="B4" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="20"/>
@@ -1337,9 +1352,9 @@
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="20"/>
@@ -1356,7 +1371,7 @@
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="1" customFormat="1">
       <c r="A6" s="21"/>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -1375,61 +1390,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="1" customFormat="1">
       <c r="A7" s="21"/>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="I7" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="8" spans="1:16">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="M9" t="b">
+      <c r="M8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="1" customFormat="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="30">
       <c r="A10" s="21"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="G10" s="14"/>
-      <c r="H10" s="14" t="b">
-        <v>0</v>
-      </c>
+      <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -1439,7 +1462,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="1" customFormat="1">
       <c r="A11" s="21"/>
       <c r="B11" s="14" t="s">
         <v>87</v>
@@ -1459,77 +1482,67 @@
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D12" s="1" t="s">
+    <row r="12" spans="1:16" s="1" customFormat="1">
+      <c r="A12" s="21"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1">
+      <c r="A13" s="21"/>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="I13" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="D14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>48</v>
       </c>
-      <c r="I12" t="s">
-        <v>146</v>
-      </c>
-      <c r="M12" t="b">
+      <c r="I14" t="s">
+        <v>144</v>
+      </c>
+      <c r="M14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-    </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
-      <c r="P14" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1">
+      <c r="A15" s="21"/>
       <c r="B15" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -1540,35 +1553,47 @@
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="15"/>
       <c r="O15" s="14"/>
-    </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14" t="s">
-        <v>140</v>
-      </c>
+      <c r="P15" s="14"/>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="D16" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>131</v>
+      </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-    </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="M16" s="14"/>
+      <c r="N16" s="15"/>
+      <c r="P16" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="14"/>
+        <v>140</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>141</v>
+      </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -1582,10 +1607,10 @@
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="14" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -1601,9 +1626,11 @@
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" s="1" customFormat="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="B19" s="14" t="s">
+        <v>142</v>
+      </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
@@ -1618,335 +1645,336 @@
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="20" spans="1:15" s="1" customFormat="1">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+    </row>
+    <row r="21" spans="1:15" s="1" customFormat="1">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+    </row>
+    <row r="22" spans="1:15" ht="22" customHeight="1">
+      <c r="B22" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="D23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>41</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F23" t="s">
         <v>49</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="4"/>
-      <c r="D23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="21"/>
       <c r="B24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A25" s="21"/>
+      <c r="B25" s="4"/>
+      <c r="D25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A26" s="21"/>
+      <c r="B26" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="4"/>
-      <c r="D26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="21"/>
       <c r="B27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A28" s="21"/>
+      <c r="B28" s="4"/>
+      <c r="D28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A29" s="21"/>
+      <c r="B29" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
-      <c r="B28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
-      <c r="B29" s="4"/>
-      <c r="D29" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="21"/>
       <c r="B30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A31" s="21"/>
+      <c r="B31" s="4"/>
+      <c r="D31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A32" s="21"/>
+      <c r="B32" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
-      <c r="B31" s="4" t="s">
+    <row r="33" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="21"/>
+      <c r="B33" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D32" s="1" t="s">
+    <row r="34" spans="1:9">
+      <c r="D34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E34" t="s">
         <v>53</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="4" t="s">
+    <row r="35" spans="1:9">
+      <c r="B35" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="D36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E36" t="s">
         <v>31</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F36" t="s">
         <v>40</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="21"/>
-      <c r="B35" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
-      <c r="B36" s="4"/>
-      <c r="D36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="21"/>
       <c r="B37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A38" s="21"/>
+      <c r="B38" s="4"/>
+      <c r="D38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A39" s="21"/>
+      <c r="B39" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
-      <c r="B38" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
-      <c r="B39" s="4"/>
-      <c r="D39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="21"/>
       <c r="B40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A41" s="21"/>
+      <c r="B41" s="4"/>
+      <c r="D41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A42" s="21"/>
+      <c r="B42" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="21"/>
-      <c r="B41" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
-      <c r="B42" s="4"/>
-      <c r="D42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="21"/>
       <c r="B43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A44" s="21"/>
+      <c r="B44" s="4"/>
+      <c r="D44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A45" s="21"/>
+      <c r="B45" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
-      <c r="B44" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
-      <c r="B45" s="4"/>
-      <c r="D45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A46" s="21"/>
       <c r="B46" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A47" s="21"/>
+      <c r="B47" s="4"/>
+      <c r="D47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A48" s="21"/>
+      <c r="B48" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="21"/>
-      <c r="B47" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="21"/>
-      <c r="B48" s="4"/>
-    </row>
-    <row r="49" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A49" s="21"/>
       <c r="B49" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A50" s="21"/>
+      <c r="B50" s="4"/>
+    </row>
+    <row r="51" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A51" s="21"/>
+      <c r="B51" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D50" s="1" t="s">
+    <row r="52" spans="1:16">
+      <c r="D52" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E52" t="s">
         <v>32</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F52" t="s">
         <v>56</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="21"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14" t="b">
+    <row r="53" spans="1:16" s="1" customFormat="1">
+      <c r="A53" s="21"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-    </row>
-    <row r="52" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D53" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E53" t="s">
-        <v>110</v>
-      </c>
-      <c r="I53" t="s">
-        <v>111</v>
-      </c>
+      <c r="I53" s="14"/>
       <c r="J53" s="14"/>
       <c r="K53" s="14"/>
-    </row>
-    <row r="54" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+    </row>
+    <row r="54" spans="1:16" s="1" customFormat="1">
       <c r="A54" s="21"/>
       <c r="B54" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>158</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -1961,41 +1989,26 @@
       <c r="O54" s="14"/>
       <c r="P54" s="14"/>
     </row>
-    <row r="55" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="21"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="J55" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K55" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="M55" s="14"/>
-      <c r="N55" s="15"/>
-      <c r="P55" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
+    <row r="55" spans="1:16">
+      <c r="D55" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E55" t="s">
+        <v>108</v>
+      </c>
+      <c r="I55" t="s">
+        <v>109</v>
+      </c>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+    </row>
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1">
+      <c r="A56" s="21"/>
       <c r="B56" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
@@ -2006,35 +2019,47 @@
       <c r="J56" s="14"/>
       <c r="K56" s="14"/>
       <c r="L56" s="14"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="15"/>
       <c r="O56" s="14"/>
-    </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14" t="s">
-        <v>140</v>
-      </c>
+      <c r="P56" s="14"/>
+    </row>
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1">
+      <c r="A57" s="21"/>
+      <c r="B57" s="14"/>
       <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
+      <c r="D57" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>131</v>
+      </c>
       <c r="F57" s="14"/>
       <c r="G57" s="14"/>
       <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-    </row>
-    <row r="58" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I57" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="K57" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="M57" s="14"/>
+      <c r="N57" s="15"/>
+      <c r="P57" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="A58" s="14"/>
       <c r="B58" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="C58" s="14"/>
+        <v>140</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>141</v>
+      </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
@@ -2048,10 +2073,10 @@
       <c r="N58" s="14"/>
       <c r="O58" s="14"/>
     </row>
-    <row r="59" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1">
       <c r="A59" s="14"/>
       <c r="B59" s="14" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
@@ -2067,20 +2092,63 @@
       <c r="N59" s="14"/>
       <c r="O59" s="14"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D60" s="1" t="s">
+    <row r="60" spans="1:16" s="1" customFormat="1">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="14"/>
+    </row>
+    <row r="61" spans="1:16" s="1" customFormat="1">
+      <c r="A61" s="14"/>
+      <c r="B61" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="14"/>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="D62" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E62" t="s">
         <v>33</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I62" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2092,7 +2160,7 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
@@ -2100,7 +2168,7 @@
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2114,7 +2182,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2126,7 +2194,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2138,7 +2206,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2150,12 +2218,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2166,7 +2234,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="10" t="s">
         <v>56</v>
       </c>
@@ -2178,7 +2246,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2189,12 +2257,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2206,7 +2274,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2218,7 +2286,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2230,7 +2298,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2242,54 +2310,59 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B16" s="3" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="10" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -2300,7 +2373,7 @@
     <col min="8" max="8" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -2320,13 +2393,13 @@
         <v>20</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="52" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>47</v>
       </c>
@@ -2345,12 +2418,12 @@
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -2362,21 +2435,21 @@
         <v>6</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -2388,96 +2461,140 @@
         <v>6</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>118</v>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="18.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="18.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2489,38 +2606,43 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="170.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
         <v>155</v>
-      </c>
-      <c r="B2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2532,13 +2654,13 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="22" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="22" customFormat="1" ht="24.5" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
@@ -2546,26 +2668,26 @@
         <v>8</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -2573,6 +2695,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2584,14 +2711,14 @@
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2602,7 +2729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2610,7 +2737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2618,7 +2745,7 @@
         <v>20140331</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2626,7 +2753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -2634,7 +2761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="11" t="s">
         <v>95</v>
       </c>
@@ -2645,18 +2772,23 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
@@ -2664,7 +2796,7 @@
     <col min="5" max="5" width="138.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -2681,7 +2813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -2695,10 +2827,10 @@
         <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2706,33 +2838,21 @@
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" t="s">
         <v>106</v>
-      </c>
-      <c r="D4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Visit tables max changes
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegan/Documents/app-designer/app/config/tables/visit/forms/visit/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="1760" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="1140" yWindow="1760" windowWidth="48120" windowHeight="25060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,18 +23,18 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="182">
   <si>
     <t>setting_name</t>
   </si>
@@ -391,9 +396,6 @@
     <t>async_assign_max</t>
   </si>
   <si>
-    <t>max_sample</t>
-  </si>
-  <si>
     <t>assign</t>
   </si>
   <si>
@@ -511,12 +513,6 @@
     <t>data('ack_ok') || calculates.below_max_height()</t>
   </si>
   <si>
-    <t>The value you entered is outside of the current recorded range 0 thru {{data.max_height}}</t>
-  </si>
-  <si>
-    <t>The value you entered is outside of the current recorded range 0 thru {{data.max_yield}}</t>
-  </si>
-  <si>
     <t>plant_type</t>
   </si>
   <si>
@@ -566,6 +562,24 @@
   </si>
   <si>
     <t>data('plant_type_query_text')</t>
+  </si>
+  <si>
+    <t>max_height_disp</t>
+  </si>
+  <si>
+    <t>max_yield_disp</t>
+  </si>
+  <si>
+    <t>data('max_height')*1.2</t>
+  </si>
+  <si>
+    <t>data('max_yield')*1.2</t>
+  </si>
+  <si>
+    <t>The value you entered is outside of the current recorded range 0 thru {{data.max_height_disp}}</t>
+  </si>
+  <si>
+    <t>The value you entered is outside of the current recorded range 0 thru {{data.max_yield_disp}}</t>
   </si>
 </sst>
 </file>
@@ -1222,19 +1236,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="76.6640625" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
@@ -1243,9 +1257,9 @@
     <col min="12" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>12</v>
@@ -1272,7 +1286,7 @@
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>110</v>
@@ -1284,19 +1298,19 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1">
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21"/>
       <c r="B2" s="14"/>
       <c r="C2" s="16"/>
       <c r="D2" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
@@ -1308,19 +1322,19 @@
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21"/>
       <c r="B3" s="14"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -1332,10 +1346,10 @@
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21"/>
       <c r="B4" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="20"/>
@@ -1352,9 +1366,9 @@
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="20"/>
@@ -1371,7 +1385,7 @@
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1">
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -1390,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1">
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>86</v>
@@ -1398,7 +1412,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1412,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1">
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -1420,10 +1434,10 @@
         <v>119</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="b">
@@ -1438,18 +1452,18 @@
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="30">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -1462,7 +1476,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1">
+    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="14" t="s">
         <v>87</v>
@@ -1482,15 +1496,15 @@
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1">
+    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14" t="s">
@@ -1506,113 +1520,118 @@
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1">
+    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
-      <c r="D13" s="1" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="I13" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="I14" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>48</v>
       </c>
-      <c r="I14" t="s">
-        <v>144</v>
-      </c>
-      <c r="M14" t="b">
+      <c r="I15" t="s">
+        <v>143</v>
+      </c>
+      <c r="M15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1">
-      <c r="A15" s="21"/>
-      <c r="B15" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-    </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="E16" s="14" t="s">
+      <c r="B16" s="14" t="s">
         <v>131</v>
       </c>
+      <c r="C16" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>159</v>
-      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
       <c r="M16" s="14"/>
       <c r="N16" s="15"/>
-      <c r="P16" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>130</v>
+      </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-    </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1">
+      <c r="I17" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M17" s="14"/>
+      <c r="N17" s="15"/>
+      <c r="P17" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="14"/>
+        <v>139</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
@@ -1626,10 +1645,10 @@
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="1:15" s="1" customFormat="1">
+    <row r="19" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -1645,10 +1664,10 @@
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="1:15" s="1" customFormat="1">
+    <row r="20" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -1664,9 +1683,11 @@
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="1:15" s="1" customFormat="1">
+    <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="B21" s="14" t="s">
+        <v>142</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -1681,305 +1702,302 @@
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="1:15" ht="22" customHeight="1">
-      <c r="B22" t="s">
+    <row r="22" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+    </row>
+    <row r="23" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>41</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>49</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A24" s="21"/>
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21"/>
+      <c r="B25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A25" s="21"/>
-      <c r="B25" s="4"/>
-      <c r="D25" s="1" t="s">
+    <row r="26" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="21"/>
+      <c r="B26" s="4"/>
+      <c r="D26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A26" s="21"/>
-      <c r="B26" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="27" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21"/>
       <c r="B27" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
+      <c r="B28" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A28" s="21"/>
-      <c r="B28" s="4"/>
-      <c r="D28" s="1" t="s">
+    <row r="29" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="21"/>
+      <c r="B29" s="4"/>
+      <c r="D29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="30" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21"/>
       <c r="B30" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="21"/>
+      <c r="B31" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="21"/>
-      <c r="B31" s="4"/>
-      <c r="D31" s="1" t="s">
+    <row r="32" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="21"/>
+      <c r="B32" s="4"/>
+      <c r="D32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A32" s="21"/>
-      <c r="B32" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21"/>
       <c r="B33" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="21"/>
+      <c r="B34" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="D34" s="1" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>53</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>31</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>40</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="21"/>
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="21"/>
+      <c r="B38" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A38" s="21"/>
-      <c r="B38" s="4"/>
-      <c r="D38" s="1" t="s">
+    <row r="39" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+      <c r="B39" s="4"/>
+      <c r="D39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A39" s="21"/>
-      <c r="B39" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="21"/>
       <c r="B40" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="21"/>
+      <c r="B41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A41" s="21"/>
-      <c r="B41" s="4"/>
-      <c r="D41" s="1" t="s">
+    <row r="42" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="21"/>
+      <c r="B42" s="4"/>
+      <c r="D42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A42" s="21"/>
-      <c r="B42" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="43" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="21"/>
       <c r="B43" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="21"/>
+      <c r="B44" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A44" s="21"/>
-      <c r="B44" s="4"/>
-      <c r="D44" s="1" t="s">
+    <row r="45" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="21"/>
+      <c r="B45" s="4"/>
+      <c r="D45" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A45" s="21"/>
-      <c r="B45" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21"/>
       <c r="B46" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="21"/>
+      <c r="B47" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A47" s="21"/>
-      <c r="B47" s="4"/>
-      <c r="D47" s="1" t="s">
+    <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="21"/>
+      <c r="B48" s="4"/>
+      <c r="D48" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A48" s="21"/>
-      <c r="B48" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="49" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="21"/>
       <c r="B49" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="21"/>
+      <c r="B50" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A50" s="21"/>
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="51" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="21"/>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="4"/>
+    </row>
+    <row r="52" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+      <c r="B52" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
-      <c r="D52" s="1" t="s">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>32</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
         <v>56</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I53" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="1" customFormat="1">
-      <c r="A53" s="21"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14" t="s">
+    <row r="54" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="21"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E53" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="F53" s="14" t="s">
+      <c r="E54" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14" t="b">
+      <c r="F54" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
-    </row>
-    <row r="54" spans="1:16" s="1" customFormat="1">
-      <c r="A54" s="21"/>
-      <c r="B54" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
       <c r="K54" s="14"/>
@@ -1989,31 +2007,40 @@
       <c r="O54" s="14"/>
       <c r="P54" s="14"/>
     </row>
-    <row r="55" spans="1:16">
-      <c r="D55" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E55" t="s">
-        <v>108</v>
-      </c>
-      <c r="I55" t="s">
-        <v>109</v>
-      </c>
+    <row r="55" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="21"/>
+      <c r="B55" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
       <c r="J55" s="14"/>
       <c r="K55" s="14"/>
-    </row>
-    <row r="56" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1">
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+    </row>
+    <row r="56" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="21"/>
-      <c r="B56" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>177</v>
+      </c>
       <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
+      <c r="G56" s="14" t="s">
+        <v>179</v>
+      </c>
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
@@ -2024,41 +2051,26 @@
       <c r="O56" s="14"/>
       <c r="P56" s="14"/>
     </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1">
-      <c r="A57" s="21"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="E57" s="14" t="s">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D57" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E57" t="s">
+        <v>108</v>
+      </c>
+      <c r="I57" t="s">
+        <v>109</v>
+      </c>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+    </row>
+    <row r="58" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="21"/>
+      <c r="B58" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="J57" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="K57" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="M57" s="14"/>
-      <c r="N57" s="15"/>
-      <c r="P57" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14" t="s">
-        <v>140</v>
-      </c>
       <c r="C58" s="14" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
@@ -2069,35 +2081,47 @@
       <c r="J58" s="14"/>
       <c r="K58" s="14"/>
       <c r="L58" s="14"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="14"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="15"/>
       <c r="O58" s="14"/>
-    </row>
-    <row r="59" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14" t="s">
-        <v>138</v>
-      </c>
+      <c r="P58" s="14"/>
+    </row>
+    <row r="59" spans="1:16" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="21"/>
+      <c r="B59" s="14"/>
       <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
+      <c r="D59" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>130</v>
+      </c>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="14"/>
-      <c r="O59" s="14"/>
-    </row>
-    <row r="60" spans="1:16" s="1" customFormat="1">
+      <c r="I59" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="J59" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="K59" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="M59" s="14"/>
+      <c r="N59" s="15"/>
+      <c r="P59" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
       <c r="B60" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C60" s="14"/>
+        <v>139</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -2111,10 +2135,10 @@
       <c r="N60" s="14"/>
       <c r="O60" s="14"/>
     </row>
-    <row r="61" spans="1:16" s="1" customFormat="1">
+    <row r="61" spans="1:16" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
       <c r="B61" s="14" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -2130,25 +2154,58 @@
       <c r="N61" s="14"/>
       <c r="O61" s="14"/>
     </row>
-    <row r="62" spans="1:16">
-      <c r="D62" s="1" t="s">
+    <row r="62" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="14"/>
+      <c r="B62" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="14"/>
+    </row>
+    <row r="63" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="14"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D64" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E64" t="s">
         <v>33</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I64" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2160,7 +2217,7 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
@@ -2168,7 +2225,7 @@
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2182,7 +2239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2194,7 +2251,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2206,7 +2263,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2218,12 +2275,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2234,7 +2291,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>56</v>
       </c>
@@ -2246,7 +2303,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2257,12 +2314,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2274,7 +2331,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2286,7 +2343,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2298,7 +2355,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2310,47 +2367,42 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C15" s="3" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C17" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2362,7 +2414,7 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -2373,7 +2425,7 @@
     <col min="8" max="8" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -2393,13 +2445,13 @@
         <v>20</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="52" customHeight="1">
+    <row r="2" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>47</v>
       </c>
@@ -2421,9 +2473,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -2447,9 +2499,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -2473,9 +2525,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2487,26 +2539,21 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H5" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="F5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2518,71 +2565,71 @@
       <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" customHeight="1">
+    <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.5" customHeight="1">
+    <row r="2" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>102</v>
@@ -2590,11 +2637,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2606,61 +2648,56 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="170.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>153</v>
       </c>
-      <c r="B2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>154</v>
-      </c>
-      <c r="B3" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="22" customFormat="1" ht="24.5" customHeight="1">
+    <row r="1" spans="1:3" s="22" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
@@ -2668,38 +2705,77 @@
         <v>8</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" t="s">
-        <v>146</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2711,14 +2787,14 @@
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2729,7 +2805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2737,7 +2813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2745,7 +2821,7 @@
         <v>20140331</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2753,7 +2829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -2761,7 +2837,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>95</v>
       </c>
@@ -2772,11 +2848,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2784,11 +2855,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
@@ -2796,7 +2867,7 @@
     <col min="5" max="5" width="138.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -2813,7 +2884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -2830,7 +2901,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2849,10 +2920,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Crop height image addition
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1760" windowWidth="48120" windowHeight="25060" tabRatio="500"/>
+    <workbookView xWindow="23340" yWindow="460" windowWidth="27680" windowHeight="26740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="183">
   <si>
     <t>setting_name</t>
   </si>
@@ -580,6 +580,9 @@
   </si>
   <si>
     <t>The value you entered is outside of the current recorded range 0 thru {{data.max_yield_disp}}</t>
+  </si>
+  <si>
+    <t>media/measure.jpg</t>
   </si>
 </sst>
 </file>
@@ -1238,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1255,6 +1258,7 @@
     <col min="9" max="10" width="59.1640625" customWidth="1"/>
     <col min="11" max="11" width="50.5" customWidth="1"/>
     <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="14" max="14" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1296,6 +1300,9 @@
       </c>
       <c r="M1" s="1" t="s">
         <v>113</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1572,6 +1579,9 @@
       </c>
       <c r="M15" t="b">
         <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Acknowledge page fix and plot report background
</commit_message>
<xml_diff>
--- a/app/config/tables/visit/forms/visit/visit.xlsx
+++ b/app/config/tables/visit/forms/visit/visit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23340" yWindow="460" windowWidth="27680" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="1320" yWindow="460" windowWidth="49700" windowHeight="26740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="186">
   <si>
     <t>setting_name</t>
   </si>
@@ -504,9 +504,6 @@
     <t>! calculates.below_max_yield()</t>
   </si>
   <si>
-    <t>data('ack_ok') || calculates.below_max_yield()</t>
-  </si>
-  <si>
     <t>! calculates.below_max_height()</t>
   </si>
   <si>
@@ -583,6 +580,18 @@
   </si>
   <si>
     <t>media/measure.jpg</t>
+  </si>
+  <si>
+    <t>The yield you have entered is an outlier.  Are you certain of this measurement?</t>
+  </si>
+  <si>
+    <t>ack_ok_2</t>
+  </si>
+  <si>
+    <t>data('ack_ok_2') || calculates.below_max_yield()</t>
+  </si>
+  <si>
+    <t>! data('ack_ok_2')</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1464,13 +1473,13 @@
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>169</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>170</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -1511,11 +1520,11 @@
         <v>120</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -1535,11 +1544,11 @@
         <v>120</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
@@ -1557,14 +1566,14 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G14" s="7"/>
       <c r="I14" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1581,7 +1590,7 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1590,7 +1599,7 @@
         <v>131</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -1623,10 +1632,10 @@
         <v>133</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M17" s="14"/>
       <c r="N17" s="15"/>
@@ -2045,11 +2054,11 @@
         <v>120</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
@@ -2104,19 +2113,19 @@
         <v>132</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
       <c r="I59" s="14" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="J59" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K59" s="14" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="M59" s="14"/>
       <c r="N59" s="15"/>
@@ -2130,7 +2139,7 @@
         <v>139</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
@@ -2379,35 +2388,35 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2537,7 +2546,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2549,16 +2558,16 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" t="s">
         <v>171</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>172</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="23" t="s">
         <v>173</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2639,7 +2648,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>102</v>
@@ -2695,10 +2704,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2731,10 +2740,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -2742,7 +2751,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
         <v>123</v>
@@ -2753,7 +2762,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>123</v>
@@ -2764,7 +2773,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
         <v>123</v>
@@ -2773,14 +2782,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>169</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>151</v>
       </c>
       <c r="B7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" t="s">
         <v>102</v>
       </c>
-      <c r="C7" t="b">
+      <c r="C8" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>